<commit_message>
fix: make subtraction work from loaded data
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t xml:space="preserve">Card Name</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">Text of card</t>
   </si>
   <si>
+    <t xml:space="preserve">When</t>
+  </si>
+  <si>
     <t xml:space="preserve">Swipe Left Text</t>
   </si>
   <si>
@@ -73,6 +76,9 @@
     <t xml:space="preserve">This is the initial card</t>
   </si>
   <si>
+    <t xml:space="preserve">environment</t>
+  </si>
+  <si>
     <t xml:space="preserve">Do the left</t>
   </si>
   <si>
@@ -106,7 +112,10 @@
     <t xml:space="preserve">Disapprove</t>
   </si>
   <si>
-    <t xml:space="preserve">A+1; Time+1</t>
+    <t xml:space="preserve">A+1; Time+1; environment-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A+1; Time+1; environment+10</t>
   </si>
   <si>
     <t xml:space="preserve">At church</t>
@@ -127,7 +136,10 @@
     <t xml:space="preserve">Decline</t>
   </si>
   <si>
-    <t xml:space="preserve">B+1; Time+1</t>
+    <t xml:space="preserve">B+1; Time+1; money-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B+1; Time+1; money+10</t>
   </si>
   <si>
     <t xml:space="preserve">At school</t>
@@ -320,15 +332,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="12.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="34.32"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -359,10 +372,10 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
@@ -370,120 +383,126 @@
       </c>
       <c r="M1" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="H2" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="J2" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="0" t="s">
         <v>22</v>
       </c>
+      <c r="K2" s="0" t="s">
+        <v>23</v>
+      </c>
       <c r="M2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>29</v>
+      <c r="K3" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>36</v>
+      <c r="K4" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add initial parsing of world queries from data
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -76,7 +76,7 @@
     <t xml:space="preserve">This is the initial card</t>
   </si>
   <si>
-    <t xml:space="preserve">environment</t>
+    <t xml:space="preserve">environment=0-100,Init=0-0</t>
   </si>
   <si>
     <t xml:space="preserve">Do the left</t>
@@ -160,6 +160,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -182,12 +183,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -334,12 +337,14 @@
   </sheetPr>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="45.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="34.32"/>
   </cols>

</xml_diff>

<commit_message>
chore: add test data with flags
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t xml:space="preserve">Card Name</t>
   </si>
@@ -76,13 +76,16 @@
     <t xml:space="preserve">This is the initial card</t>
   </si>
   <si>
-    <t xml:space="preserve">environment=0-100,Init=0-0</t>
+    <t xml:space="preserve">environment=0-100,Init=0-0;test=true</t>
   </si>
   <si>
     <t xml:space="preserve">Do the left</t>
   </si>
   <si>
     <t xml:space="preserve">Do the right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Init+1;Time=0; test=true; apa=false</t>
   </si>
   <si>
     <t xml:space="preserve">Init+1;Time=0</t>
@@ -338,10 +341,10 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="45.71"/>
@@ -419,95 +422,95 @@
         <v>21</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J3" s="0" t="s">
         <v>14</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J4" s="0" t="s">
         <v>14</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add support for loading card weight from data
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
   <si>
     <t xml:space="preserve">Card Name</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weight</t>
   </si>
   <si>
     <t xml:space="preserve">initial_card</t>
@@ -338,18 +341,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O4" activeCellId="0" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="45.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="34.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="32.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="40.29"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -395,122 +398,134 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="O2" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="K3" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="O3" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>23</v>
-      </c>
       <c r="M4" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="O4" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: add example effect to data
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="init" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="sequence1" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -92,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="209">
   <si>
     <t xml:space="preserve">Card Name</t>
   </si>
@@ -244,6 +245,9 @@
     <t xml:space="preserve">Build a solar farm</t>
   </si>
   <si>
+    <t xml:space="preserve">money-10</t>
+  </si>
+  <si>
     <t xml:space="preserve">UI_TestWind</t>
   </si>
   <si>
@@ -256,6 +260,9 @@
     <t xml:space="preserve">Congratulations! You have built a wind farm</t>
   </si>
   <si>
+    <t xml:space="preserve">Environment+10; popularity+10</t>
+  </si>
+  <si>
     <t xml:space="preserve">UI_Test_3</t>
   </si>
   <si>
@@ -338,6 +345,381 @@
   </si>
   <si>
     <t xml:space="preserve">Yes, I am ready to play!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_Intro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time to make good on our promises. The Secretary of Energy wants to see you. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We'll have that meeting later. I've got more important things to do</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great. I am excited to get started</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_Windfarm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secretary of Energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good morning, governor. We promised to make big changes to our energy economy. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(continue)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_Start = False</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_Windfarm2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To get started quickly we can either build a wind far or import green energy from a neighbor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Let's be self sufficient. We should build a wind farm.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If there is green energy already available, we should just buy it from our neigbhors.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_WindfarmResult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excellent. I'll get started on it right away.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_WindfarmLeft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Economic Advisor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We've started constructing turbines. The local manufacturing unions will be very happy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_WindfarmRight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Environmental NGO Rep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a representative of a green energy NGO, I am happy you found green energy without any additional construction.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_BuildLocation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secretary of Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We're ready to begin construction on our new wind farm. We can build a coastal or an interior farm.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windfarm_Built = True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_BuildLocation2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coastal farms produce less but are easier to manage. Interior farms require land but will create jobs near former mines.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Build a coastal windfarm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Build an interior wind farm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_Greenbuy_Require</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opportunity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We got a great contract to import green energy. Should we require everyone use some green energy?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No. People have the right to choose between cheap or clean energy. I won't force them to go green.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes. All electricity substations should use about 20% green energy. It will be pricy, but worth the cost.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windfarm_Built = False</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_BuildLocationCoast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These wind turbines will be an eyesore on the coast. Tourism companies are starting to complain. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spread out the turbines. It will be less efficient, but look nicer.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Let's create a tourism campaign. We can make the turbines a location to visit and build a "green energy museum"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_BuildLocationInter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coal Lobbyist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I represent the coal industry. We have a power substation near your wind farm. Sharing it would save us both money.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No. We will need to build our own stations, if we want independence from coal.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">That sounds like a great plan. We need to cooperate to move forward.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_optional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Opposing Politician</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is a pretty weak commitment to green energy. You were elected to make a difference!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are doing everything we can. People understand a balance is needed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Issue a statement. We should make it clear that this is just the start.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_Required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You're requiring people to buy a product that undermines our own coal industry! We will not forget this!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I am doing exactly what I campaigned on. This is the will of the people.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">He's right. I should run an PR campaign to help people understand why we did this.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_CoastOffer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are ready to construct our coastal windfarm. Should we build it close to shore or in deeper waters? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Close to shore. That may damage the coastal ecosystem, but it will hugely help the local economy and energy efficiency.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deep waters. It's expensive and may disrupt fishing, but we need to protect the coast.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windfarm_Built = True, Windfarm_Coast = True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_InterOffer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time to build our interior wind farm. Should we use public land or subsidize building on private land?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Public land. We can build near highways. This will be more expensive, but much more efficient.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subsidize. We can ask farmers to use their empty farmland. This is cheaper to maintain, but will produce less energy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windfarm_Built = True, Windfarm_Coast = False</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_Priorities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The green energy cost is becoming a financial burden for some. Should we help small businesses or the needy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Small businesses. They spend a lot of money on electricity. If they lose money, we lose jobs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The needy. We can't askfamilies to leave the heater off to save money!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windfarm_built = False, Greenbuy_Require = True</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_Incentivize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The optional green energy is much more expensive. People won't use it, if it's too costly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We can't fix every problem at once. We gave people the choice. They will need to follow their heart.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If we offer a subsidized discount for the first few months, it will encourage people to switch to green.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windfarm_built = False, Greenbuy_Require = False</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_Coast_Shallow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The turbines are degrading the coastal ecosystem. The government has to do something.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We can't afford a restoration project. The energy is worth damage to the coast.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The energy isn't worth it, if the coast is destroyed. I'll fund a coastal restoration project.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_Coast_Deep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The wind turbines are impacting fishing. Boat captains say the waters are too crowded now. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expand the commercial fishing season so boats have more months they can be out. That should reduce traffic. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is an opportunity to reduce our fishing impact. Reduce the number of commercial fishing licenses we issue.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_Inter_Farm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Local Politician</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I represent one of the farming towns you built turbines in. The turbines are drying the air. Crops are dying!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The area the turbines affect is very small. If we reduce the number of turbines, it will be fine.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Different crops will grow better in the dryer area. Changing will be an expensive process, though.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_Inter_State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secretary of Transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We have cheap land for turbines near the highways, but people hate seeing wind farms near roads.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Build near the highway. People need cheap energy more than they need pretty roads.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Build on hidden land. We don't want people angry at the green energy projects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_businessfirst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The business lobby was very appreciative of our policies and wants to donate to our reelection campaign.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No. We can't be seen taking big donations. We want to appear fair and unbiased.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This will go a long way to helping us get reelected. The longer we stay in office, the more good we can do!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_familyfirst</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your energy policy helped a lot of families this year. Should we build a PR campaign to show how much it helped?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No. I don't want to appear like I did it just for the good press. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes. We can use some good will. An interview will highlight how energy policy helps people.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_incentives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The governor  is using your tax money to pay other people's bills. Time for a change! </t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Don't respond. You don't want to get dragged into a public debate.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We use taxpayer money to fund thousands of programs like education. Green energy is the will of the people.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_noincentives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not many people are using the green option. We could start converting government buildings to green energy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No. We should focus on making the energy publicly available.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great idea. Start switching over public buildings immediately.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_Sellwind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A neighboring state is offering to buy most of our wind energy. This would recoup much of the money we spent.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No. If we sell our wind energy, all of this was for nothing.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes. This will be a long road. We will need the money to keep developing more green energy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_Shutcoal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">With wind and coal plants we have an excess of energy. Should we sell some or shut down one of our coal plants?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sell the energy. We keep our coal industry workers employed and can fund future green energy projects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shut the plant down. It will be difficult, but that's the ultimate goal. Best to get started.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_Sold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think you made the right decision. We will need the money in the future.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_Nosale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think you made the right choice. We just spent a lot of money on building green energy. Why sell it?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_Noshut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think you made the right choice. We can't risk all those jobs until we have a much stronger green economy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S1_shutitdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think you made the right choice. The sooner we start converting to green energy, the sooner our jobs market can adjust</t>
   </si>
 </sst>
 </file>
@@ -347,7 +729,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -393,13 +775,33 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -410,6 +812,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -447,7 +855,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -474,6 +882,18 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -555,8 +975,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2:L26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1039,11 +1459,17 @@
       <c r="F14" s="5" t="s">
         <v>49</v>
       </c>
+      <c r="G14" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="I14" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L14" s="0" t="s">
         <v>21</v>
@@ -1057,14 +1483,14 @@
     </row>
     <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>18</v>
@@ -1072,11 +1498,17 @@
       <c r="F15" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="G15" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="I15" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L15" s="0" t="s">
         <v>21</v>
@@ -1090,26 +1522,32 @@
     </row>
     <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>18</v>
+      <c r="H16" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L16" s="0" t="s">
         <v>21</v>
@@ -1123,16 +1561,16 @@
     </row>
     <row r="17" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>18</v>
@@ -1141,10 +1579,10 @@
         <v>18</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L17" s="0" t="s">
         <v>21</v>
@@ -1158,14 +1596,14 @@
     </row>
     <row r="18" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>18</v>
@@ -1174,10 +1612,10 @@
         <v>18</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="L18" s="0" t="s">
         <v>21</v>
@@ -1191,26 +1629,26 @@
     </row>
     <row r="19" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L19" s="0" t="s">
         <v>21</v>
@@ -1224,14 +1662,14 @@
     </row>
     <row r="20" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>18</v>
@@ -1240,10 +1678,10 @@
         <v>18</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="L20" s="0" t="s">
         <v>21</v>
@@ -1257,14 +1695,14 @@
     </row>
     <row r="21" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>18</v>
@@ -1273,10 +1711,10 @@
         <v>18</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="L21" s="0" t="s">
         <v>21</v>
@@ -1290,14 +1728,14 @@
     </row>
     <row r="22" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>18</v>
@@ -1306,10 +1744,10 @@
         <v>18</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L22" s="0" t="s">
         <v>21</v>
@@ -1323,14 +1761,14 @@
     </row>
     <row r="23" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>18</v>
@@ -1339,10 +1777,10 @@
         <v>18</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="L23" s="0" t="s">
         <v>21</v>
@@ -1356,14 +1794,14 @@
     </row>
     <row r="24" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>18</v>
@@ -1372,10 +1810,10 @@
         <v>18</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="L24" s="0" t="s">
         <v>21</v>
@@ -1389,14 +1827,14 @@
     </row>
     <row r="25" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>18</v>
@@ -1405,10 +1843,10 @@
         <v>18</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="L25" s="0" t="s">
         <v>21</v>
@@ -1422,20 +1860,20 @@
     </row>
     <row r="26" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="L26" s="0" t="s">
         <v>21</v>
@@ -1467,4 +1905,842 @@
   </headerFooter>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AMJ32"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O29" activeCellId="0" sqref="O29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="62.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="34.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="51.4"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="8"/>
+    </row>
+    <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="O3" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="P3" s="8"/>
+    </row>
+    <row r="4" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="8"/>
+    </row>
+    <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="8"/>
+    </row>
+    <row r="6" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="8"/>
+    </row>
+    <row r="7" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="8"/>
+    </row>
+    <row r="8" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="O8" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="P8" s="8"/>
+    </row>
+    <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="O9" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="P9" s="8"/>
+    </row>
+    <row r="10" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="O10" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="P10" s="8"/>
+    </row>
+    <row r="11" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="8"/>
+    </row>
+    <row r="12" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="8"/>
+    </row>
+    <row r="13" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="8"/>
+    </row>
+    <row r="14" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="O14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="O15" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="O16" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="O17" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="O18" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="O19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="O20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="O21" s="5"/>
+    </row>
+    <row r="22" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="O22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="O23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="O24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="O25" s="5"/>
+    </row>
+    <row r="26" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="O26" s="5"/>
+    </row>
+    <row r="27" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="O27" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="O28" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="O29" s="5"/>
+    </row>
+    <row r="30" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="O30" s="5"/>
+    </row>
+    <row r="31" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="O31" s="5"/>
+    </row>
+    <row r="32" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="O32" s="5"/>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="B2:B32" type="list">
+      <formula1>"Offer,Result,Event,Opportunity,Focus Group"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="C2:C11 G10:H10 C12 C14:C32 G17:H18 G22:H25 G27:H32" type="list">
+      <formula1>"Economic Advisor,Campaign Advisor,Secretary of Education,Secretary of Energy,Secretary of Development,Secretary of Transport,Environmental NGO Rep,Coal Lobbyist,Opposing Politician,Local Politician,Focus Group,Environmentally Minded Citizen,Undecided Vote"&amp;"r,Coal Miner"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
chore: update example to use replace effect
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="215">
   <si>
     <t xml:space="preserve">Card Name</t>
   </si>
@@ -257,6 +257,9 @@
     <t xml:space="preserve">Result</t>
   </si>
   <si>
+    <t xml:space="preserve">Wind Farm</t>
+  </si>
+  <si>
     <t xml:space="preserve">Congratulations! You have built a wind farm</t>
   </si>
   <si>
@@ -266,6 +269,9 @@
     <t xml:space="preserve">UI_Test_3</t>
   </si>
   <si>
+    <t xml:space="preserve">Solar Farm</t>
+  </si>
+  <si>
     <t xml:space="preserve">Congratulations! You have built a solar farm</t>
   </si>
   <si>
@@ -302,6 +308,12 @@
     <t xml:space="preserve">Intro_FocusGroup_Enviro</t>
   </si>
   <si>
+    <t xml:space="preserve">Out in the wild</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presentation Round</t>
+  </si>
+  <si>
     <t xml:space="preserve">Environmentally Minded Citizen</t>
   </si>
   <si>
@@ -345,6 +357,12 @@
   </si>
   <si>
     <t xml:space="preserve">Yes, I am ready to play!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finish==0; finish==false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finish==0; finish==true</t>
   </si>
   <si>
     <t xml:space="preserve">Group</t>
@@ -729,7 +747,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -772,11 +790,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -855,7 +868,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -884,15 +897,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -975,15 +984,15 @@
   </sheetPr>
   <dimension ref="A1:AMJ26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="59.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="32.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="59.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="32.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="40.29"/>
   </cols>
   <sheetData>
@@ -1462,7 +1471,7 @@
       <c r="G14" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="6" t="s">
         <v>50</v>
       </c>
       <c r="I14" s="3" t="s">
@@ -1488,9 +1497,11 @@
       <c r="B15" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="D15" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>18</v>
@@ -1498,17 +1509,17 @@
       <c r="F15" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G15" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>55</v>
+      <c r="G15" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L15" s="0" t="s">
         <v>21</v>
@@ -1527,27 +1538,29 @@
       <c r="B16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="D16" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="J16" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L16" s="0" t="s">
         <v>21</v>
@@ -1561,7 +1574,7 @@
     </row>
     <row r="17" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>53</v>
@@ -1570,7 +1583,7 @@
         <v>16</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>18</v>
@@ -1579,10 +1592,10 @@
         <v>18</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="L17" s="0" t="s">
         <v>21</v>
@@ -1596,14 +1609,14 @@
     </row>
     <row r="18" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>18</v>
@@ -1612,10 +1625,10 @@
         <v>18</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L18" s="0" t="s">
         <v>21</v>
@@ -1629,26 +1642,26 @@
     </row>
     <row r="19" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L19" s="0" t="s">
         <v>21</v>
@@ -1662,14 +1675,14 @@
     </row>
     <row r="20" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>18</v>
@@ -1678,16 +1691,16 @@
         <v>18</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="N20" s="0" t="n">
         <v>1</v>
@@ -1695,14 +1708,14 @@
     </row>
     <row r="21" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>18</v>
@@ -1711,16 +1724,16 @@
         <v>18</v>
       </c>
       <c r="I21" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="L21" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="J21" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="L21" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="M21" s="0" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="N21" s="0" t="n">
         <v>1</v>
@@ -1728,32 +1741,32 @@
     </row>
     <row r="22" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="L22" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="M22" s="0" t="s">
         <v>72</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I22" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="L22" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M22" s="0" t="s">
-        <v>22</v>
       </c>
       <c r="N22" s="0" t="n">
         <v>1</v>
@@ -1761,14 +1774,14 @@
     </row>
     <row r="23" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>18</v>
@@ -1777,10 +1790,10 @@
         <v>18</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="L23" s="0" t="s">
         <v>21</v>
@@ -1794,14 +1807,14 @@
     </row>
     <row r="24" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>18</v>
@@ -1810,10 +1823,10 @@
         <v>18</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="L24" s="0" t="s">
         <v>21</v>
@@ -1827,14 +1840,14 @@
     </row>
     <row r="25" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>18</v>
@@ -1843,10 +1856,10 @@
         <v>18</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="L25" s="0" t="s">
         <v>21</v>
@@ -1860,20 +1873,26 @@
     </row>
     <row r="26" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>89</v>
       </c>
       <c r="L26" s="0" t="s">
         <v>21</v>
@@ -1918,7 +1937,7 @@
       <selection pane="topLeft" activeCell="O29" activeCellId="0" sqref="O29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.59"/>
@@ -1975,13 +1994,13 @@
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>46</v>
@@ -1990,222 +2009,222 @@
         <v>16</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="O2" s="5"/>
-      <c r="P2" s="8"/>
+      <c r="P2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="O3" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="P3" s="8"/>
+        <v>99</v>
+      </c>
+      <c r="P3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="O4" s="5"/>
-      <c r="P4" s="8"/>
+      <c r="P4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="O5" s="5"/>
-      <c r="P5" s="8"/>
+      <c r="P5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
-        <v>100</v>
+      <c r="A6" s="8" t="s">
+        <v>106</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="O6" s="5"/>
-      <c r="P6" s="8"/>
+      <c r="P6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
-        <v>103</v>
+      <c r="A7" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="O7" s="5"/>
-      <c r="P7" s="8"/>
+      <c r="P7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
-      <c r="O8" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="P8" s="8"/>
+      <c r="O8" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="P8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
-      <c r="O9" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="P9" s="8"/>
+      <c r="O9" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="P9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
-      <c r="O10" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="P10" s="8"/>
+      <c r="O10" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="P10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>53</v>
@@ -2214,85 +2233,85 @@
         <v>16</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="O13" s="5"/>
-      <c r="P13" s="8"/>
+      <c r="P13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -2300,122 +2319,122 @@
     </row>
     <row r="15" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
-      <c r="O15" s="9" t="s">
-        <v>143</v>
+      <c r="O15" s="8" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
-      <c r="O16" s="9" t="s">
-        <v>148</v>
+      <c r="O16" s="8" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>101</v>
-      </c>
       <c r="D17" s="5" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="O17" s="5" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="O18" s="5" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -2423,68 +2442,68 @@
     </row>
     <row r="20" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="O20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="9" t="s">
-        <v>167</v>
+      <c r="A21" s="8" t="s">
+        <v>173</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="O21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9" t="s">
-        <v>172</v>
+      <c r="A22" s="8" t="s">
+        <v>178</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
@@ -2492,7 +2511,7 @@
     </row>
     <row r="23" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>53</v>
@@ -2501,13 +2520,13 @@
         <v>16</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
@@ -2515,7 +2534,7 @@
     </row>
     <row r="24" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>53</v>
@@ -2524,13 +2543,13 @@
         <v>16</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
@@ -2538,22 +2557,22 @@
     </row>
     <row r="25" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
@@ -2561,22 +2580,22 @@
     </row>
     <row r="26" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
@@ -2584,72 +2603,72 @@
     </row>
     <row r="27" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="O27" s="5" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>46</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="O28" s="5" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
@@ -2657,22 +2676,22 @@
     </row>
     <row r="30" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
@@ -2680,22 +2699,22 @@
     </row>
     <row r="31" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
@@ -2703,22 +2722,22 @@
     </row>
     <row r="32" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>53</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>

</xml_diff>

<commit_message>
feat: add experimental daycycle to coal mining scenario
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="225">
   <si>
     <t xml:space="preserve">Card Name</t>
   </si>
@@ -140,6 +140,9 @@
     <t xml:space="preserve">When</t>
   </si>
   <si>
+    <t xml:space="preserve">Require</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hello_Player</t>
   </si>
   <si>
@@ -167,6 +170,9 @@
     <t xml:space="preserve">init=false</t>
   </si>
   <si>
+    <t xml:space="preserve">Daycycle=1-3;</t>
+  </si>
+  <si>
     <t xml:space="preserve">We have a lot of choices to make. You can choose by swiping the card left or right. Try now.</t>
   </si>
   <si>
@@ -363,6 +369,30 @@
   </si>
   <si>
     <t xml:space="preserve">Finish==0; finish==true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morning_Coffee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morning Coffee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mmm… this morning coffee is so good.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day+1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At the breakfast table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morning joy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daycycle=0-0;</t>
   </si>
   <si>
     <t xml:space="preserve">Group</t>
@@ -982,13 +1012,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ26"/>
+  <dimension ref="A1:AMJ27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H26" activeCellId="0" sqref="H26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="59.06"/>
@@ -1042,866 +1072,979 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N3" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="P3" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N4" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="P4" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N5" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="P5" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N6" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="P6" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N7" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="P7" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N8" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="P8" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N9" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="P9" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N10" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="P10" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N11" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="P11" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N12" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="P12" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N13" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="P13" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N14" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="P14" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N15" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="P15" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="H16" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>57</v>
-      </c>
       <c r="J16" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N16" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="P16" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N17" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="P17" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N18" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="P18" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N19" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="P19" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="N20" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="P20" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="L21" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="M21" s="0" t="s">
         <v>74</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="L21" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="M21" s="0" t="s">
-        <v>72</v>
       </c>
       <c r="N21" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="P21" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="N22" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="P22" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N23" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="P23" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M24" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N24" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="P24" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="J25" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N25" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="P25" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M26" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N26" s="0" t="n">
         <v>1</v>
+      </c>
+      <c r="P26" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="L27" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="M27" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="N27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O27" s="0" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1937,7 +2080,7 @@
       <selection pane="topLeft" activeCell="O29" activeCellId="0" sqref="O29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.59"/>
@@ -1994,28 +2137,28 @@
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
@@ -2024,48 +2167,48 @@
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="O3" s="5" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="P3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -2074,22 +2217,22 @@
     </row>
     <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -2098,22 +2241,22 @@
     </row>
     <row r="6" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="D6" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>98</v>
-      </c>
       <c r="F6" s="5" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
@@ -2122,22 +2265,22 @@
     </row>
     <row r="7" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -2146,100 +2289,100 @@
     </row>
     <row r="8" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="O8" s="8" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="P8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="O9" s="8" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="P9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="O10" s="8" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="P10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -2248,22 +2391,22 @@
     </row>
     <row r="12" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
@@ -2272,22 +2415,22 @@
     </row>
     <row r="13" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
@@ -2296,22 +2439,22 @@
     </row>
     <row r="14" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -2319,122 +2462,122 @@
     </row>
     <row r="15" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="O15" s="8" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="O16" s="8" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="O17" s="5" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="O18" s="5" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -2442,22 +2585,22 @@
     </row>
     <row r="20" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
@@ -2465,22 +2608,22 @@
     </row>
     <row r="21" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
@@ -2488,22 +2631,22 @@
     </row>
     <row r="22" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
@@ -2511,22 +2654,22 @@
     </row>
     <row r="23" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
@@ -2534,22 +2677,22 @@
     </row>
     <row r="24" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
@@ -2557,22 +2700,22 @@
     </row>
     <row r="25" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
@@ -2580,22 +2723,22 @@
     </row>
     <row r="26" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
@@ -2603,72 +2746,72 @@
     </row>
     <row r="27" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="O27" s="5" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="O28" s="5" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
@@ -2676,22 +2819,22 @@
     </row>
     <row r="30" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
@@ -2699,22 +2842,22 @@
     </row>
     <row r="31" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
@@ -2722,22 +2865,22 @@
     </row>
     <row r="32" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>

</xml_diff>

<commit_message>
feat: add more experimental content to breakfast philosophy
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="238">
   <si>
     <t xml:space="preserve">Card Name</t>
   </si>
@@ -377,10 +377,13 @@
     <t xml:space="preserve">Morning Coffee</t>
   </si>
   <si>
-    <t xml:space="preserve">Mmm… this morning coffee is so good.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start day</t>
+    <t xml:space="preserve">The coffee tastes unusually good today. But is it really sustainable to be enjoying it in this part of the world?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A day needs a good start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perhaps not</t>
   </si>
   <si>
     <t xml:space="preserve">Day+1</t>
@@ -389,10 +392,46 @@
     <t xml:space="preserve">At the breakfast table</t>
   </si>
   <si>
-    <t xml:space="preserve">Morning joy</t>
+    <t xml:space="preserve">Breakfast philosophy</t>
   </si>
   <si>
     <t xml:space="preserve">Daycycle=0-0;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are so many conflicting parties in environmental politics. How should I convince my opposition?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Push harder and act stronger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listen, understand and discuss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I really need to get to the office soon. Should I really take the car?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use the subway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Take the towncar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This ham sandwich. I love it. But can I continue eating it? Can I find an alternative?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try smoked paprika</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is not that much anyways</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The public seems to not understand the importance of my politics. Maybe I need to focus on something else.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maybe just a few more tax cuts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stay on target. Focus on the environment</t>
   </si>
   <si>
     <t xml:space="preserve">Group</t>
@@ -1012,18 +1051,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ27"/>
+  <dimension ref="A1:AMJ31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N28" activeCellId="0" sqref="N28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="59.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="32.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="40.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="22.09"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2026,25 +2066,165 @@
         <v>95</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="L27" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="M27" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="N27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O27" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="G28" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="M27" s="0" t="s">
+      <c r="H28" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="L28" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="N27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="O27" s="0" t="s">
+      <c r="M28" s="0" t="s">
         <v>99</v>
+      </c>
+      <c r="N28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O28" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="F29" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="L29" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="M29" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="N29" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O29" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="F30" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="G30" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="L30" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="M30" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="N30" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O30" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="G31" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="L31" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="M31" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="N31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="O31" s="0" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2080,7 +2260,7 @@
       <selection pane="topLeft" activeCell="O29" activeCellId="0" sqref="O29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.59"/>
@@ -2137,13 +2317,13 @@
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>48</v>
@@ -2152,13 +2332,13 @@
         <v>17</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
@@ -2167,48 +2347,48 @@
     </row>
     <row r="3" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="O3" s="5" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="P3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -2217,22 +2397,22 @@
     </row>
     <row r="5" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -2241,22 +2421,22 @@
     </row>
     <row r="6" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
@@ -2265,22 +2445,22 @@
     </row>
     <row r="7" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>108</v>
-      </c>
       <c r="F7" s="5" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -2289,85 +2469,85 @@
     </row>
     <row r="8" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="O8" s="8" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="P8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="O9" s="8" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="P9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="O10" s="8" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="P10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>55</v>
@@ -2376,13 +2556,13 @@
         <v>17</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -2391,22 +2571,22 @@
     </row>
     <row r="12" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
@@ -2415,22 +2595,22 @@
     </row>
     <row r="13" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
@@ -2439,22 +2619,22 @@
     </row>
     <row r="14" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -2462,122 +2642,122 @@
     </row>
     <row r="15" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="O15" s="8" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="O16" s="8" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="O17" s="5" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="O18" s="5" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -2585,22 +2765,22 @@
     </row>
     <row r="20" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
@@ -2608,22 +2788,22 @@
     </row>
     <row r="21" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
@@ -2631,22 +2811,22 @@
     </row>
     <row r="22" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
@@ -2654,7 +2834,7 @@
     </row>
     <row r="23" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>55</v>
@@ -2663,13 +2843,13 @@
         <v>17</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>194</v>
+        <v>207</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
@@ -2677,7 +2857,7 @@
     </row>
     <row r="24" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>55</v>
@@ -2686,13 +2866,13 @@
         <v>17</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>199</v>
+        <v>212</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
@@ -2700,22 +2880,22 @@
     </row>
     <row r="25" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
@@ -2723,22 +2903,22 @@
     </row>
     <row r="26" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5" t="s">
-        <v>205</v>
+        <v>218</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>207</v>
+        <v>220</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>208</v>
+        <v>221</v>
       </c>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
@@ -2746,72 +2926,72 @@
     </row>
     <row r="27" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5" t="s">
-        <v>209</v>
+        <v>222</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>211</v>
+        <v>224</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>212</v>
+        <v>225</v>
       </c>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
       <c r="O27" s="5" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>213</v>
+        <v>226</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>48</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>214</v>
+        <v>227</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>216</v>
+        <v>229</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="O28" s="5" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>217</v>
+        <v>230</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>218</v>
+        <v>231</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
@@ -2819,22 +2999,22 @@
     </row>
     <row r="30" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5" t="s">
-        <v>219</v>
+        <v>232</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>220</v>
+        <v>233</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
@@ -2842,22 +3022,22 @@
     </row>
     <row r="31" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5" t="s">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
@@ -2865,22 +3045,22 @@
     </row>
     <row r="32" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>223</v>
+        <v>236</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>55</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>224</v>
+        <v>237</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>

</xml_diff>